<commit_message>
Word Break - Part 2
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C759D1EB-9D59-4E53-845A-7019C6C0D164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4CBD3D-6B1D-4FBC-BB26-E68AB07D242A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="C276" sqref="C276"/>
+      <selection activeCell="C277" sqref="C277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4764,7 +4764,7 @@
         <v>268</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="21">

</xml_diff>

<commit_message>
stack implemented from scratch
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4CBD3D-6B1D-4FBC-BB26-E68AB07D242A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135A2434-6365-497B-9887-56D8F3A72F52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="C277" sqref="C277"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="C296" sqref="C296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4959,7 +4959,7 @@
         <v>286</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Middle Element in stack
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0AA060-6DCE-4B79-B392-4C4C3C78119F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB970CF3-93FD-43BF-B9AD-2D7C0E21B522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="C298" sqref="C298"/>
+      <selection activeCell="C299" sqref="C299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4992,7 +4992,7 @@
         <v>289</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Reverse a string using Stack
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3509B3F8-6B3A-40EF-A318-6A9269890D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC343534-F613-439A-9834-F5FECDBCC948}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+      <selection activeCell="C302" sqref="C302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5025,7 +5025,7 @@
         <v>292</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Insert an element at its bottom without using any other datastructure
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65E71F2-553B-44AB-A9BE-1D352FECE34A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17A76FC-B484-4643-B01C-DCFDC3C3EC6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="C305" sqref="C305"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="C308" sqref="C308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5091,7 +5091,7 @@
         <v>298</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Sort a Stack Using Recursion
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE10802-8365-4887-937E-F9C58A74D942}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6879C6B0-2916-4299-ADDC-B1A43A8D696A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="C309" sqref="C309"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5113,7 +5113,7 @@
         <v>300</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Maximum Rectangular Area in a Histogram
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57308A3-07BF-4452-A450-E37ED289F93A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4872539-C9E3-4C52-8480-3135D8991E33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="C311" sqref="C311"/>
+    <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
+      <selection activeCell="C312" sqref="C312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5135,7 +5135,7 @@
         <v>302</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Evaluation of Postfix Expression
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0F8E5A-7474-4538-84E2-1B95572322FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C5E646-C00D-45DD-8FBE-CBB5BB3EF369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="C306" sqref="C306"/>
+      <selection activeCell="C307" sqref="C307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5080,7 +5080,7 @@
         <v>297</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Expression contains redundant bracket or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE856B5-977A-4AAA-B656-3A35D9D37848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01588612-ED4A-4A6D-877F-627E9CF71636}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="C313" sqref="C313"/>
+      <selection activeCell="C314" sqref="C314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5157,7 +5157,7 @@
         <v>304</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Stack using two queues
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01588612-ED4A-4A6D-877F-627E9CF71636}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2353C70E-4558-43F0-9333-C6FDB827E86B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="C314" sqref="C314"/>
+      <selection activeCell="C315" sqref="C315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5168,7 +5168,7 @@
         <v>305</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Implement Stack and Queue using Deque
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2353C70E-4558-43F0-9333-C6FDB827E86B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9553DDF1-A642-43F9-8184-90ED790CB946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="C315" sqref="C315"/>
+      <selection activeCell="C316" sqref="C316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5179,7 +5179,7 @@
         <v>306</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Stack Permutations (Check if an array is stack permutation of other)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9553DDF1-A642-43F9-8184-90ED790CB946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3649A52-D436-4807-AEDC-011A994514C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="C316" sqref="C316"/>
+    <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
+      <selection activeCell="C317" sqref="C317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5190,7 +5190,7 @@
         <v>307</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Queue using two Stacks
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3649A52-D436-4807-AEDC-011A994514C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0796D2-AA96-4368-8A1C-6BD0A04BE955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
-      <selection activeCell="C317" sqref="C317"/>
+      <selection activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5201,7 +5201,7 @@
         <v>308</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Reverse Queue using Recursion
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C272B22-BF2C-41C8-882C-B304B216D048}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0838DAB-FA3F-448E-AD70-F53582702081}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="C320" sqref="C320"/>
+    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="C323" sqref="C323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5245,7 +5245,7 @@
         <v>312</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="21">
@@ -5256,7 +5256,7 @@
         <v>313</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Interleave the first half of the queue with second half
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0838DAB-FA3F-448E-AD70-F53582702081}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFA20A2-4A15-44BA-B4B5-ADB3FB437C15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="C323" sqref="C323"/>
+      <selection activeCell="C324" sqref="C324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5267,7 +5267,7 @@
         <v>314</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Distance of nearest cell having 1
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB494B33-F262-4C91-8AD4-3306BF8A63A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5ADD37-FB60-4D6F-BB7A-9F921BBE5E53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
-      <selection activeCell="B326" sqref="B326"/>
+      <selection activeCell="C327" sqref="C327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5300,7 +5300,7 @@
         <v>317</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="21">

</xml_diff>

<commit_message>
First negative integer in every window of size k
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5ADD37-FB60-4D6F-BB7A-9F921BBE5E53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11FCA86-CCCA-409E-A660-2D9F50E66AD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
-      <selection activeCell="C327" sqref="C327"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="C328" sqref="C328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5311,7 +5311,7 @@
         <v>318</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Check if all levels of two trees are anagrams or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11FCA86-CCCA-409E-A660-2D9F50E66AD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01145137-DC8E-42C3-999A-2DEDEF9430C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="C328" sqref="C328"/>
+      <selection activeCell="C329" sqref="C329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5322,7 +5322,7 @@
         <v>319</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find the first non-repeating character from a stream of characters
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01145137-DC8E-42C3-999A-2DEDEF9430C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F752DD-087E-4E1F-8646-62ECD5827A26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="C329" sqref="C329"/>
+      <selection activeCell="C332" sqref="C332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5355,7 +5355,7 @@
         <v>322</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="333" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Median in a row-wise sorted Matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392769A6-9CE9-4536-9CB0-93ACE0394D16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30836E8A-05BB-4ED2-ADA6-F59DDF1E3635}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2333,7 +2333,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find a specific pair in Matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4743D50A-EBC7-45E9-8950-165017015AB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6770AB7-AEE3-4135-A963-77F7F2E59346}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2377,7 +2377,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Roatae Matrix By 90 degree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6770AB7-AEE3-4135-A963-77F7F2E59346}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844D5C43-5CFB-496B-B4FC-F4EA24E2945E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2388,7 +2388,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Common elements in all rows of a given matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844D5C43-5CFB-496B-B4FC-F4EA24E2945E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CF09B3-E156-4D7F-94BE-B894F9152B27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2410,7 +2410,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Maximum of all subarrays of size k
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A3C192-CA86-409A-A390-0BD6443058E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEA52A2-471B-47A0-83E7-89C1316ED03F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="C337" sqref="C337"/>
+      <selection activeCell="C338" sqref="C338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5407,7 +5407,7 @@
         <v>327</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Merge k Sorted Arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924E81FD-CFE5-4770-AEE6-A8B17D27DAF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7F8879-8FFC-4600-9AF5-3DEB4A4BDAE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="C340" sqref="C340"/>
+      <selection activeCell="C341" sqref="C341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5440,7 +5440,7 @@
         <v>330</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Merge two binary Max Heaps
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7F8879-8FFC-4600-9AF5-3DEB4A4BDAE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A921E5-E744-4E33-85B1-9822B2867F0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="C341" sqref="C341"/>
+    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
+      <selection activeCell="C342" sqref="C342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5451,7 +5451,7 @@
         <v>331</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="21">

</xml_diff>

<commit_message>
K-th Largest Sum Contiguous Subarray
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A921E5-E744-4E33-85B1-9822B2867F0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB8CBBE-2620-4B97-ABE9-FE06B2379B08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="C342" sqref="C342"/>
+      <selection activeCell="C343" sqref="C343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5462,7 +5462,7 @@
         <v>332</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Merged K Sorted Linked Lists using Heap
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB8CBBE-2620-4B97-ABE9-FE06B2379B08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C331D98A-838E-41D3-AFA1-21BA4882FAAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="C343" sqref="C343"/>
+      <selection activeCell="C345" sqref="C345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5484,7 +5484,7 @@
         <v>334</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Smallest range in K lists
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C331D98A-838E-41D3-AFA1-21BA4882FAAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB7F6FC-E370-4C57-A311-967A54EE7746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="C345" sqref="C345"/>
+      <selection activeCell="C346" sqref="C346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5495,7 +5495,7 @@
         <v>335</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="347" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find median in a stream
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB7F6FC-E370-4C57-A311-967A54EE7746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F251A02-E679-4B54-B064-99DC8108BEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="C346" sqref="C346"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="C347" sqref="C347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5506,7 +5506,7 @@
         <v>336</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="348" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Is Binary Tree Heap
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F251A02-E679-4B54-B064-99DC8108BEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC237E0-D56F-4F83-B311-2BA64FC82463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="C347" sqref="C347"/>
+      <selection activeCell="C348" sqref="C348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5517,7 +5517,7 @@
         <v>337</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Convert BST to minHeap
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B1D805-C6FB-403E-BAFB-D60A906B6BC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7BECF9-43F8-4161-929A-9000D990DA08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="C349" sqref="C349"/>
+    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
+      <selection activeCell="C350" sqref="C350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5539,7 +5539,7 @@
         <v>339</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="351" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Convert min Heap to max Heap
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7BECF9-43F8-4161-929A-9000D990DA08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC90F6E-4CE9-46D9-9134-E34515D835AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="C350" sqref="C350"/>
+    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="C351" sqref="C351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5550,7 +5550,7 @@
         <v>340</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="352" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Kth element in Matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF409B-B589-40B9-B478-FB2B4964A020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A35F51D-0A71-4B56-A575-B24A93DCA44A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="C352" sqref="C352"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2399,7 +2399,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="21">

</xml_diff>

<commit_message>
create Graph and print
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A35F51D-0A71-4B56-A575-B24A93DCA44A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AEB0A8-3166-48AD-9C1E-3406557BF72C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="C356" sqref="C356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5591,7 +5591,7 @@
         <v>344</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Detect cycle in an undirected graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518801C1-9C2F-4363-B13B-65849E24288B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89BC8D4-0E8E-4429-A1A6-58C818DBB3FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="C357" sqref="C357"/>
+      <selection activeCell="C360" sqref="C360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5635,7 +5635,7 @@
         <v>348</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Detect cycle in a directed graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89BC8D4-0E8E-4429-A1A6-58C818DBB3FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B04FBA3-DFCA-48B3-BFDB-45DEF5BE1739}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="C360" sqref="C360"/>
+      <selection activeCell="C359" sqref="C359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5624,7 +5624,7 @@
         <v>347</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Rat in a Maze Problem - I
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B04FBA3-DFCA-48B3-BFDB-45DEF5BE1739}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE8EA8-924D-41DC-A93D-9215528F8729}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="C359" sqref="C359"/>
+      <selection activeCell="C361" sqref="C361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5646,7 +5646,7 @@
         <v>349</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Dijkstra’s shortest path algorithm
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93957AA-5480-42FA-AEB5-4869884AB5E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3716A688-791B-4418-8416-2952641BDD2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="C368" sqref="C368"/>
+    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="C367" sqref="C367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5712,7 +5712,7 @@
         <v>355</v>
       </c>
       <c r="C367" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Find the number of islands
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B282CF1-610B-4812-8BD5-F9599E039109}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC283ED-D620-454C-A04A-3555C9F488D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
-      <selection activeCell="C370" sqref="C370"/>
+      <selection activeCell="C371" sqref="C371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5756,7 +5756,7 @@
         <v>359</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="21">

</xml_diff>